<commit_message>
update sugar unity version
</commit_message>
<xml_diff>
--- a/Assets/SUGAR/Resources/Localization/SUGAR Unity Localization.xlsx
+++ b/Assets/SUGAR/Resources/Localization/SUGAR Unity Localization.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\Projects\sugar-unity\Unity\Assets\SUGAR\Resources\Localization\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="510" yWindow="600" windowWidth="24615" windowHeight="11955"/>
+    <workbookView xWindow="510" yWindow="600" windowWidth="24620" windowHeight="11960"/>
   </bookViews>
   <sheets>
     <sheet name="SUGARLocalizations" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
   <si>
     <t>Key</t>
   </si>
@@ -269,6 +274,12 @@
   </si>
   <si>
     <t>Alliances</t>
+  </si>
+  <si>
+    <t>REMEMBER</t>
+  </si>
+  <si>
+    <t>Remember Me</t>
   </si>
 </sst>
 </file>
@@ -324,6 +335,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -371,7 +385,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -406,7 +420,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,22 +629,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.7265625" customWidth="1"/>
     <col min="2" max="2" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +661,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -664,7 +678,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -681,7 +695,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -698,7 +712,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -715,7 +729,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -732,7 +746,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -749,7 +763,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -766,7 +780,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -783,7 +797,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -800,7 +814,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -817,7 +831,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -834,7 +848,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -851,7 +865,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -868,7 +882,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -885,7 +899,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -902,7 +916,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -919,7 +933,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -936,7 +950,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -953,7 +967,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -970,7 +984,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
@@ -987,7 +1001,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -1004,7 +1018,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
@@ -1021,7 +1035,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
@@ -1038,7 +1052,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -1055,7 +1069,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>48</v>
       </c>
@@ -1072,7 +1086,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
@@ -1089,7 +1103,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>52</v>
       </c>
@@ -1106,7 +1120,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
@@ -1123,7 +1137,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
@@ -1140,7 +1154,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>58</v>
       </c>
@@ -1157,7 +1171,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>60</v>
       </c>
@@ -1174,7 +1188,7 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>62</v>
       </c>
@@ -1191,7 +1205,7 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
@@ -1208,12 +1222,12 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>67</v>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1225,12 +1239,12 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1242,12 +1256,12 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1259,12 +1273,12 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1276,12 +1290,12 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1293,12 +1307,12 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1310,12 +1324,12 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1327,19 +1341,36 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>